<commit_message>
Move files, redesign file structure, create sprint blog and brainstorming
</commit_message>
<xml_diff>
--- a/Docs/Backlog.xlsx
+++ b/Docs/Backlog.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stallman\Source\Repos\SaNi\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint #1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="0">Backlog!$A$2</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="91">
   <si>
     <t>Configuration</t>
   </si>
@@ -150,6 +151,156 @@
   </si>
   <si>
     <t>Platform independent graphics wrapper that hides implementation details</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Filesystem</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>Wrappers</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Reading &amp; Writing</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Timers</t>
+  </si>
+  <si>
+    <t>DirectX 11</t>
+  </si>
+  <si>
+    <t>OpenGL 3</t>
+  </si>
+  <si>
+    <t>OpenGLES 2</t>
+  </si>
+  <si>
+    <t>Voidbab</t>
+  </si>
+  <si>
+    <t>Study how D3D works; Testing and stuff;</t>
+  </si>
+  <si>
+    <t>GraphicsDevice</t>
+  </si>
+  <si>
+    <t>siquel</t>
+  </si>
+  <si>
+    <t>XML</t>
+  </si>
+  <si>
+    <t>Vectors</t>
+  </si>
+  <si>
+    <t>Matrices</t>
+  </si>
+  <si>
+    <t>Quaternions</t>
+  </si>
+  <si>
+    <t>Rectangles</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Voidbab &amp; siquel</t>
+  </si>
+  <si>
+    <t>Sum up after sprint</t>
+  </si>
+  <si>
+    <t>Should be pretty straightforward;</t>
+  </si>
+  <si>
+    <t>Same as with D3D</t>
+  </si>
+  <si>
+    <t>Load files</t>
+  </si>
+  <si>
+    <t>Create var lists</t>
+  </si>
+  <si>
+    <t>Typedefs</t>
+  </si>
+  <si>
+    <t>Stopwatch</t>
+  </si>
+  <si>
+    <t>Callback timer</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Not assigned</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Logging features</t>
+  </si>
+  <si>
+    <t>Console logger</t>
+  </si>
+  <si>
+    <t>File logger</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Vector 2, 3 and 4</t>
+  </si>
+  <si>
+    <t>Matrix 2, 3 and 4</t>
+  </si>
+  <si>
+    <t>Rotations</t>
+  </si>
+  <si>
+    <t>AABB's and basic functions</t>
+  </si>
+  <si>
+    <t>Helpers, randoms</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Problems</t>
   </si>
 </sst>
 </file>
@@ -165,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +335,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -208,11 +407,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -225,6 +450,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,4 +1108,410 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>42178</v>
+      </c>
+      <c r="B2" s="18">
+        <v>42185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="F5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="F6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>